<commit_message>
Ny DB conn funktion
</commit_message>
<xml_diff>
--- a/Projekt Beskrivningar/Reports/Time report.xlsx
+++ b/Projekt Beskrivningar/Reports/Time report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\DagbokProjekt\Projekt Beskrivningar\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AE9D49D-8627-424C-B4A7-6FEC35A93175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD70D70-8FCF-4145-A04A-C2690B92640E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{F7BFEC0F-D3D6-47A9-94FC-57DB3F8A7DB4}"/>
+    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="11385" xr2:uid="{F7BFEC0F-D3D6-47A9-94FC-57DB3F8A7DB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>TIDSREDOVISNING</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t>Interface</t>
+  </si>
+  <si>
+    <t>Databas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -412,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83B938FA-C183-4B88-AE19-B1C1AB776B71}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,17 +430,17 @@
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -445,12 +451,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>44942</v>
       </c>
@@ -458,7 +464,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>44944</v>
       </c>
@@ -466,7 +472,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>44949</v>
       </c>
@@ -474,10 +480,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -488,31 +494,45 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
         <v>44951</v>
       </c>
       <c r="C11">
+        <v>75</v>
+      </c>
+      <c r="F11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="2">
+        <v>44951</v>
+      </c>
+      <c r="C15">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C12">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C16">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C13">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C14">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C15">
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C19">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Glömd Push från 30/01
Försöker få Ta bort att fungera som det skall.
</commit_message>
<xml_diff>
--- a/Projekt Beskrivningar/Reports/Time report.xlsx
+++ b/Projekt Beskrivningar/Reports/Time report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\DagbokProjekt\Projekt Beskrivningar\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4469E8F-EAC1-4C84-B9BC-AAA17D83E888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F426A529-7E7B-44A0-9C16-E5FD57103391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4200" yWindow="2595" windowWidth="21600" windowHeight="11385" xr2:uid="{F7BFEC0F-D3D6-47A9-94FC-57DB3F8A7DB4}"/>
+    <workbookView xWindow="-25320" yWindow="270" windowWidth="25440" windowHeight="15390" xr2:uid="{F7BFEC0F-D3D6-47A9-94FC-57DB3F8A7DB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>TIDSREDOVISNING</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>(Häma,Skicka,Koppla)</t>
   </si>
 </sst>
 </file>
@@ -421,7 +424,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,10 +508,16 @@
         <v>7</v>
       </c>
     </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="3"/>
+    </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>6</v>
-      </c>
       <c r="B15" s="2">
         <v>44951</v>
       </c>
@@ -521,47 +530,51 @@
         <v>44952</v>
       </c>
       <c r="C16">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="2">
+        <v>44956</v>
+      </c>
       <c r="C17">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C18">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C19">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C21">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C22">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>15</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="B14:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>